<commit_message>
exercise1ai.py: total number of bits implemented, number of different symbols almost there
</commit_message>
<xml_diff>
--- a/module2/Relatorio/exercicio1-ab-i.xlsx
+++ b/module2/Relatorio/exercicio1-ab-i.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micae\Desktop\CD-Pratica\module2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micae\Desktop\CD-Pratica\module2\Relatorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C847210-883F-4CFC-BF27-C533A1AD28B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA70CBD-34E6-47C5-A007-9A480768C288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{E92FA622-30D8-4DED-9AD9-B9524BD83BAD}"/>
+    <workbookView xWindow="-20610" yWindow="1890" windowWidth="20730" windowHeight="11160" xr2:uid="{E92FA622-30D8-4DED-9AD9-B9524BD83BAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
     <t>p</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>Erro (%)</t>
+  </si>
+  <si>
+    <t>Exercício 1 a) i)</t>
+  </si>
+  <si>
+    <t>Exercício 1 b) i)</t>
   </si>
 </sst>
 </file>
@@ -64,11 +70,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="171" formatCode="0.00000"/>
-    <numFmt numFmtId="172" formatCode="0.000000"/>
-    <numFmt numFmtId="173" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,6 +90,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -112,12 +126,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF8DDF49-39F7-4754-9E66-9578C9E43D01}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -453,268 +473,322 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="E3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="I3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="M3" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+    </row>
+    <row r="4" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O4" s="5" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="B3" s="3">
-        <v>9.9699999999999997E-2</v>
-      </c>
-      <c r="C3" s="4">
-        <f>(B3-A3)/A3</f>
-        <v>-3.0000000000000859E-3</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F3" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="G3" s="4">
-        <f>(F3-E3)/E3</f>
-        <v>0</v>
-      </c>
-      <c r="I3" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="J3" s="3">
-        <v>9.9199999999999997E-2</v>
-      </c>
-      <c r="K3" s="4">
-        <f>(J3-I3)/I3</f>
-        <v>-8.0000000000000904E-3</v>
-      </c>
-      <c r="M3" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="N3" s="3">
-        <v>9.9900000000000003E-2</v>
-      </c>
-      <c r="O3" s="4">
-        <f>(N3-M3)/M3</f>
-        <v>-1.0000000000000286E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="B4" s="3">
-        <v>9.2399999999999999E-3</v>
-      </c>
-      <c r="C4" s="4">
-        <f t="shared" ref="C4:C7" si="0">(B4-A4)/A4</f>
-        <v>-7.6000000000000026E-2</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="F4" s="3">
-        <v>9.8499999999999994E-3</v>
-      </c>
-      <c r="G4" s="4">
-        <f t="shared" ref="G4:G7" si="1">(F4-E4)/E4</f>
-        <v>-1.5000000000000083E-2</v>
-      </c>
-      <c r="I4" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="J4" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="K4" s="4">
-        <f t="shared" ref="K4:K7" si="2">(J4-I4)/I4</f>
-        <v>0</v>
-      </c>
-      <c r="M4" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="N4" s="3">
-        <v>9.9000000000000008E-3</v>
-      </c>
-      <c r="O4" s="4">
-        <f t="shared" ref="O4:O7" si="3">(N4-M4)/M4</f>
-        <v>-9.9999999999999395E-3</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="B5" s="3">
+        <v>9.9699999999999997E-2</v>
+      </c>
+      <c r="C5" s="4">
+        <f>(B5-A5)/A5</f>
+        <v>-3.0000000000000859E-3</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G5" s="4">
+        <f>(F5-E5)/E5</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="J5" s="3">
+        <v>9.9199999999999997E-2</v>
+      </c>
+      <c r="K5" s="4">
+        <f>(J5-I5)/I5</f>
+        <v>-8.0000000000000904E-3</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="N5" s="3">
+        <v>9.9900000000000003E-2</v>
+      </c>
+      <c r="O5" s="4">
+        <f>(N5-M5)/M5</f>
+        <v>-1.0000000000000286E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="B6" s="3">
+        <v>9.2399999999999999E-3</v>
+      </c>
+      <c r="C6" s="4">
+        <f t="shared" ref="C6:C9" si="0">(B6-A6)/A6</f>
+        <v>-7.6000000000000026E-2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="F6" s="3">
+        <v>9.8499999999999994E-3</v>
+      </c>
+      <c r="G6" s="4">
+        <f t="shared" ref="G6:G9" si="1">(F6-E6)/E6</f>
+        <v>-1.5000000000000083E-2</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="K6" s="4">
+        <f t="shared" ref="K6:K9" si="2">(J6-I6)/I6</f>
+        <v>0</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="N6" s="3">
+        <v>9.9000000000000008E-3</v>
+      </c>
+      <c r="O6" s="4">
+        <f t="shared" ref="O6:O9" si="3">(N6-M6)/M6</f>
+        <v>-9.9999999999999395E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>1E-3</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B7" s="3">
         <v>7.6999999999999996E-4</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C7" s="4">
         <f t="shared" si="0"/>
         <v>-0.23000000000000007</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E7" s="2">
         <v>1E-3</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F7" s="3">
         <v>9.810000000000001E-4</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G7" s="4">
         <f t="shared" si="1"/>
         <v>-1.899999999999992E-2</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I7" s="2">
         <v>1E-3</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J7" s="3">
         <v>1.1100000000000001E-3</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K7" s="4">
         <f t="shared" si="2"/>
         <v>0.11000000000000007</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M7" s="2">
         <v>1E-3</v>
       </c>
-      <c r="N5" s="3">
+      <c r="N7" s="3">
         <v>1.14E-3</v>
       </c>
-      <c r="O5" s="4">
+      <c r="O7" s="4">
         <f t="shared" si="3"/>
         <v>0.13999999999999993</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>1E-4</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B8" s="3">
         <v>0</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C8" s="4">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E8" s="2">
         <v>1E-4</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F8" s="3">
         <v>8.2200000000000006E-5</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G8" s="4">
         <f t="shared" si="1"/>
         <v>-0.17799999999999999</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I8" s="2">
         <v>1E-4</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J8" s="3">
         <v>1.18E-4</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K8" s="4">
         <f t="shared" si="2"/>
         <v>0.17999999999999988</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M8" s="2">
         <v>1E-4</v>
       </c>
-      <c r="N6" s="3">
+      <c r="N8" s="3">
         <v>1.06E-4</v>
       </c>
-      <c r="O6" s="4">
+      <c r="O8" s="4">
         <f t="shared" si="3"/>
         <v>5.9999999999999963E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B9" s="3">
         <v>0</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C9" s="4">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E9" s="2">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F9" s="3">
         <v>1.1E-5</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G9" s="4">
         <f t="shared" si="1"/>
         <v>9.9999999999999881E-2</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I9" s="2">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J9" s="3">
         <v>1.5400000000000002E-5</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K9" s="4">
         <f t="shared" si="2"/>
         <v>0.54</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M9" s="2">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="N7" s="3">
+      <c r="N9" s="3">
         <v>6.3999999999999997E-6</v>
       </c>
-      <c r="O7" s="4">
+      <c r="O9" s="4">
         <f t="shared" si="3"/>
         <v>-0.3600000000000001</v>
       </c>
     </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+    </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A12:O12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>